<commit_message>
Began work for creating a new assessment
</commit_message>
<xml_diff>
--- a/Time plan.xlsx
+++ b/Time plan.xlsx
@@ -640,7 +640,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1044,9 @@
       <c r="E17" s="20">
         <v>2</v>
       </c>
-      <c r="F17" s="20"/>
+      <c r="F17" s="20">
+        <v>8</v>
+      </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
@@ -1058,7 +1060,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More work on tree view integration
+ Context menu for nodes
+ All buttons working
+ Insert above/below
+ Move up/down
+ Delete
+Expand/collapse list
</commit_message>
<xml_diff>
--- a/Time plan.xlsx
+++ b/Time plan.xlsx
@@ -640,7 +640,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1047,9 @@
       <c r="F17" s="20">
         <v>8</v>
       </c>
-      <c r="G17" s="20"/>
+      <c r="G17" s="20">
+        <v>6</v>
+      </c>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
@@ -1060,7 +1062,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
most text editor functions now work
</commit_message>
<xml_diff>
--- a/Time plan.xlsx
+++ b/Time plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -640,28 +640,28 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="40.33203125" customWidth="1"/>
-    <col min="3" max="15" width="8.6640625" customWidth="1"/>
-    <col min="18" max="18" width="8.88671875" style="17"/>
+    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="3" max="15" width="8.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="17"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>10</v>
       </c>
@@ -715,7 +715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="25"/>
       <c r="B7" s="26"/>
       <c r="C7" s="4"/>
@@ -735,7 +735,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="19"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -764,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="12" t="s">
         <v>5</v>
@@ -791,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>2</v>
       </c>
@@ -822,7 +822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
         <v>5</v>
@@ -853,7 +853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>3</v>
       </c>
@@ -910,7 +910,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="12" t="s">
         <v>5</v>
@@ -941,7 +941,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
         <v>4</v>
       </c>
@@ -972,7 +972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="12" t="s">
         <v>5</v>
@@ -999,7 +999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>5</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="12" t="s">
         <v>5</v>
@@ -1065,7 +1065,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>6</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="12" t="s">
         <v>5</v>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>7</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="12" t="s">
         <v>5</v>
@@ -1168,7 +1168,9 @@
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="H21" s="20">
+        <v>17</v>
+      </c>
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
@@ -1180,10 +1182,10 @@
       <c r="Q21" s="20"/>
       <c r="R21" s="20">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
         <v>10</v>
       </c>
@@ -1214,7 +1216,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="12" t="s">
         <v>5</v>
@@ -1239,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>11</v>
       </c>
@@ -1266,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="12" t="s">
         <v>5</v>
@@ -1291,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>12</v>
       </c>
@@ -1318,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="12" t="s">
         <v>5</v>
@@ -1343,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -1363,7 +1365,7 @@
       <c r="Q28"/>
       <c r="R28" s="17"/>
     </row>
-    <row r="29" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -1383,7 +1385,7 @@
       <c r="Q29"/>
       <c r="R29" s="17"/>
     </row>
-    <row r="30" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -1403,7 +1405,7 @@
       <c r="Q30"/>
       <c r="R30" s="17"/>
     </row>
-    <row r="31" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -1423,7 +1425,7 @@
       <c r="Q31"/>
       <c r="R31" s="17"/>
     </row>
-    <row r="32" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>

</xml_diff>

<commit_message>
Examinee GUI design work
</commit_message>
<xml_diff>
--- a/Time plan.xlsx
+++ b/Time plan.xlsx
@@ -96,16 +96,16 @@
     <t>Design of Assessment Designer GUI</t>
   </si>
   <si>
-    <t>Design of Examiner GUI</t>
-  </si>
-  <si>
-    <t>Backend programming for Examiner</t>
-  </si>
-  <si>
     <t>Backend programming for Assessment Designer</t>
   </si>
   <si>
     <t>Semester 1 2016</t>
+  </si>
+  <si>
+    <t>Design of Examinee GUI</t>
+  </si>
+  <si>
+    <t>Backend programming for Examinee</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -658,7 +658,7 @@
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -924,21 +924,39 @@
       <c r="E13" s="20">
         <v>0.5</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="F13" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="20">
+        <v>0.5</v>
+      </c>
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
+      <c r="L13" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="M13" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="N13" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="O13" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="P13" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="20">
+        <v>0.5</v>
+      </c>
       <c r="R13" s="20">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -946,7 +964,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22">
@@ -988,7 +1006,9 @@
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
+      <c r="L15" s="20">
+        <v>3</v>
+      </c>
       <c r="M15" s="20"/>
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
@@ -996,7 +1016,7 @@
       <c r="Q15" s="20"/>
       <c r="R15" s="20">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1070,7 +1090,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
@@ -1126,7 +1146,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
@@ -1172,8 +1192,12 @@
         <v>17</v>
       </c>
       <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
+      <c r="J21" s="20">
+        <v>2</v>
+      </c>
+      <c r="K21" s="20">
+        <v>1</v>
+      </c>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
       <c r="N21" s="20"/>
@@ -1182,7 +1206,7 @@
       <c r="Q21" s="20"/>
       <c r="R21" s="20">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>